<commit_message>
Remove unused event fields from QcFmRecord model and clean up related forms. Fix the navbar issue
</commit_message>
<xml_diff>
--- a/qcfm/static/qcfm/QC_FM.xlsx
+++ b/qcfm/static/qcfm/QC_FM.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="10440"/>
+    <workbookView windowWidth="23040" windowHeight="9995"/>
   </bookViews>
   <sheets>
     <sheet name="QC" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>QUALITY CONTROL FOCAL MECHANISM</t>
   </si>
@@ -54,12 +54,6 @@
   </si>
   <si>
     <t>: Kel. 1</t>
-  </si>
-  <si>
-    <t>Event di Indonesia: 3</t>
-  </si>
-  <si>
-    <t>Event di Luar Negeri: 1</t>
   </si>
   <si>
     <t>No</t>
@@ -1378,7 +1372,7 @@
   <dimension ref="B1:R990"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I$1:I$1048576"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4259259259259" defaultRowHeight="15" customHeight="1"/>
@@ -1473,16 +1467,12 @@
       <c r="N5" s="21"/>
     </row>
     <row r="6" ht="23.4" customHeight="1" spans="2:14">
-      <c r="B6" s="5" t="s">
-        <v>9</v>
-      </c>
+      <c r="B6" s="5"/>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
-      <c r="G6" s="5" t="s">
-        <v>10</v>
-      </c>
+      <c r="G6" s="5"/>
       <c r="H6" s="5"/>
       <c r="I6" s="5"/>
       <c r="J6" s="5"/>
@@ -1493,53 +1483,53 @@
     </row>
     <row r="7" ht="18" customHeight="1" spans="2:18">
       <c r="B7" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="E7" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="F7" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="G7" s="8" t="s">
         <v>14</v>
-      </c>
-      <c r="F7" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="G7" s="8" t="s">
-        <v>16</v>
       </c>
       <c r="H7" s="9"/>
       <c r="I7" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="J7" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="K7" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="J7" s="8" t="s">
+      <c r="L7" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="K7" s="22" t="s">
+      <c r="M7" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="L7" s="8" t="s">
+      <c r="N7" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="M7" s="8" t="s">
+      <c r="O7" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="N7" s="8" t="s">
+      <c r="P7" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="O7" s="8" t="s">
+      <c r="Q7" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="P7" s="8" t="s">
+      <c r="R7" s="8" t="s">
         <v>24</v>
-      </c>
-      <c r="Q7" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="R7" s="8" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="8" ht="14.4" customHeight="1" spans="2:14">
@@ -1576,7 +1566,7 @@
       <c r="B10" s="10"/>
       <c r="C10" s="13"/>
       <c r="D10" s="14" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E10" s="13"/>
       <c r="F10" s="10"/>
@@ -1587,7 +1577,7 @@
       <c r="K10" s="11"/>
       <c r="L10" s="10"/>
       <c r="M10" s="14" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="N10" s="10"/>
     </row>
@@ -1595,7 +1585,7 @@
       <c r="B11" s="10"/>
       <c r="C11" s="15"/>
       <c r="D11" s="16" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E11" s="14"/>
       <c r="F11" s="10"/>
@@ -1606,7 +1596,7 @@
       <c r="K11" s="11"/>
       <c r="L11" s="10"/>
       <c r="M11" s="14" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="N11" s="10"/>
     </row>
@@ -1674,7 +1664,7 @@
       <c r="B16" s="10"/>
       <c r="C16" s="17"/>
       <c r="D16" s="18" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E16" s="19"/>
       <c r="F16" s="10"/>
@@ -1685,7 +1675,7 @@
       <c r="K16" s="11"/>
       <c r="L16" s="10"/>
       <c r="M16" s="23" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="N16" s="10"/>
     </row>
@@ -1693,7 +1683,7 @@
       <c r="B17" s="10"/>
       <c r="C17" s="17"/>
       <c r="D17" s="16" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E17" s="20"/>
       <c r="F17" s="10"/>
@@ -1704,7 +1694,7 @@
       <c r="K17" s="11"/>
       <c r="L17" s="10"/>
       <c r="M17" s="20" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="N17" s="10"/>
     </row>

</xml_diff>